<commit_message>
Slight changes to lists
</commit_message>
<xml_diff>
--- a/Data/Skyros List.xlsx
+++ b/Data/Skyros List.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eranee\Desktop\Beetles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eranee\Desktop\Beetles\RScripts\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DD4F63-8630-43EE-AA93-2165A074355A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B3767D-5C54-4184-A5CE-CA57FC1FC243}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{983DCE97-DC4A-4F6A-9F48-E813D0A7A667}"/>
   </bookViews>
@@ -424,7 +424,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,6 +436,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -461,10 +468,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,13 +787,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3126BC85-CBBC-4973-B6A7-AA5644100AFA}">
-  <dimension ref="A1:AT84"/>
+  <dimension ref="A1:AU84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AB58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AD57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AU85" sqref="AU85"/>
+      <selection pane="bottomRight" activeCell="AU84" sqref="AU84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,7 +805,7 @@
     <col min="25" max="25" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>69</v>
       </c>
@@ -931,7 +939,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -944,7 +952,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1085,8 +1093,12 @@
         <f>SUM(Z3:AS3)</f>
         <v>0</v>
       </c>
+      <c r="AU3">
+        <f>SUM(Y3,AT3)</f>
+        <v>32</v>
+      </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1227,8 +1239,12 @@
         <f t="shared" ref="AT4:AT67" si="0">SUM(Z4:AS4)</f>
         <v>0</v>
       </c>
+      <c r="AU4">
+        <f t="shared" ref="AU4:AU67" si="1">SUM(Y4,AT4)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1243,8 +1259,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1385,8 +1405,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1527,8 +1551,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU7">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1669,8 +1697,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1811,8 +1843,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1825,8 +1861,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1967,8 +2007,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1981,8 +2025,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2056,7 +2104,7 @@
         <v>12</v>
       </c>
       <c r="Y13">
-        <f t="shared" ref="Y13:Y20" si="1">SUM(C13:X13)</f>
+        <f t="shared" ref="Y13:Y20" si="2">SUM(C13:X13)</f>
         <v>11</v>
       </c>
       <c r="Z13" t="s">
@@ -2123,8 +2171,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU13">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -2198,7 +2250,7 @@
         <v>3</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="Z14" t="s">
@@ -2265,8 +2317,12 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
+      <c r="AU14">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -2340,7 +2396,7 @@
         <v>12</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="Z15" t="s">
@@ -2407,8 +2463,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU15">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
@@ -2482,7 +2542,7 @@
         <v>1</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="Z16" t="s">
@@ -2549,8 +2609,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="AU16">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
@@ -2624,7 +2688,7 @@
         <v>12</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="Z17" t="s">
@@ -2691,8 +2755,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU17">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>110</v>
       </c>
@@ -2829,8 +2897,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="AU18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
@@ -2904,7 +2976,7 @@
         <v>12</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="Z19" t="s">
@@ -2971,8 +3043,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU19">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
@@ -3046,7 +3122,7 @@
         <v>12</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Z20" t="s">
@@ -3113,8 +3189,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -3123,8 +3203,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>35</v>
       </c>
@@ -3265,8 +3349,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="AU22">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
     </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -3275,8 +3363,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>37</v>
       </c>
@@ -3350,7 +3442,7 @@
         <v>12</v>
       </c>
       <c r="Y24">
-        <f t="shared" ref="Y24:Y53" si="2">SUM(C24:X24)</f>
+        <f t="shared" ref="Y24:Y53" si="3">SUM(C24:X24)</f>
         <v>1</v>
       </c>
       <c r="Z24" t="s">
@@ -3417,8 +3509,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>123</v>
       </c>
@@ -3555,8 +3651,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="AU25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
@@ -3630,7 +3730,7 @@
         <v>12</v>
       </c>
       <c r="Y26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Z26" t="s">
@@ -3697,8 +3797,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU26">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
@@ -3772,7 +3876,7 @@
         <v>12</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="Z27" t="s">
@@ -3839,8 +3943,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU27">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
     </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
@@ -3914,7 +4022,7 @@
         <v>12</v>
       </c>
       <c r="Y28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="Z28" t="s">
@@ -3981,8 +4089,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU28">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
     </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
@@ -4056,7 +4168,7 @@
         <v>1</v>
       </c>
       <c r="Y29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="Z29" t="s">
@@ -4123,8 +4235,12 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="AU29">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
     </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
@@ -4198,7 +4314,7 @@
         <v>11</v>
       </c>
       <c r="Y30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="Z30" t="s">
@@ -4265,8 +4381,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU30">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
     </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>43</v>
       </c>
@@ -4340,7 +4460,7 @@
         <v>12</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="Z31">
@@ -4407,8 +4527,12 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
+      <c r="AU31">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
     </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>44</v>
       </c>
@@ -4482,7 +4606,7 @@
         <v>12</v>
       </c>
       <c r="Y32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="Z32" t="s">
@@ -4549,8 +4673,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU32">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>45</v>
       </c>
@@ -4624,7 +4752,7 @@
         <v>2</v>
       </c>
       <c r="Y33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="Z33" t="s">
@@ -4691,9 +4819,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU33">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -4766,7 +4898,7 @@
         <v>12</v>
       </c>
       <c r="Y34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Z34" t="s">
@@ -4833,9 +4965,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU34">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -4908,7 +5044,7 @@
         <v>12</v>
       </c>
       <c r="Y35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="Z35" t="s">
@@ -4975,8 +5111,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU35">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>48</v>
       </c>
@@ -5050,7 +5190,7 @@
         <v>12</v>
       </c>
       <c r="Y36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="Z36" t="s">
@@ -5117,8 +5257,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU36">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>120</v>
       </c>
@@ -5192,7 +5336,7 @@
         <v>1</v>
       </c>
       <c r="Y37">
-        <f t="shared" ref="Y37" si="3">SUM(C37:X37)</f>
+        <f t="shared" ref="Y37" si="4">SUM(C37:X37)</f>
         <v>5</v>
       </c>
       <c r="Z37" t="s">
@@ -5259,9 +5403,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU37">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>124</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -5400,8 +5548,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="AU38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>66</v>
       </c>
@@ -5475,7 +5627,7 @@
         <v>12</v>
       </c>
       <c r="Y39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="Z39" t="s">
@@ -5542,8 +5694,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU39">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>126</v>
       </c>
@@ -5683,8 +5839,12 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
+      <c r="AU40">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
     </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>50</v>
       </c>
@@ -5758,7 +5918,7 @@
         <v>12</v>
       </c>
       <c r="Y41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="Z41" t="s">
@@ -5825,8 +5985,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU41">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>52</v>
       </c>
@@ -5900,7 +6064,7 @@
         <v>12</v>
       </c>
       <c r="Y42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Z42" t="s">
@@ -5967,8 +6131,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU42">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>125</v>
       </c>
@@ -6108,8 +6276,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="AU43">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
@@ -6183,7 +6355,7 @@
         <v>1</v>
       </c>
       <c r="Y44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="Z44" t="s">
@@ -6250,8 +6422,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU44">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
     </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>54</v>
       </c>
@@ -6325,7 +6501,7 @@
         <v>1</v>
       </c>
       <c r="Y45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="Z45" t="s">
@@ -6392,8 +6568,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="AU45">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
     </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>121</v>
       </c>
@@ -6467,7 +6647,7 @@
         <v>12</v>
       </c>
       <c r="Y46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="Z46" t="s">
@@ -6534,8 +6714,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU46">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>55</v>
       </c>
@@ -6609,7 +6793,7 @@
         <v>4</v>
       </c>
       <c r="Y47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="Z47" t="s">
@@ -6676,8 +6860,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU47">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
     </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>56</v>
       </c>
@@ -6751,7 +6939,7 @@
         <v>12</v>
       </c>
       <c r="Y48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="Z48" t="s">
@@ -6818,8 +7006,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU48">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
     </row>
-    <row r="49" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>57</v>
       </c>
@@ -6893,7 +7085,7 @@
         <v>4</v>
       </c>
       <c r="Y49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="Z49" t="s">
@@ -6960,8 +7152,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU49">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
     </row>
-    <row r="50" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>58</v>
       </c>
@@ -7035,7 +7231,7 @@
         <v>12</v>
       </c>
       <c r="Y50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Z50" t="s">
@@ -7102,8 +7298,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU50">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>59</v>
       </c>
@@ -7112,8 +7312,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU51">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>60</v>
       </c>
@@ -7187,7 +7391,7 @@
         <v>12</v>
       </c>
       <c r="Y52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>160</v>
       </c>
       <c r="Z52" t="s">
@@ -7254,8 +7458,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU52">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
     </row>
-    <row r="53" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>63</v>
       </c>
@@ -7329,7 +7537,7 @@
         <v>12</v>
       </c>
       <c r="Y53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="Z53" t="s">
@@ -7396,8 +7604,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU53">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
     </row>
-    <row r="54" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>67</v>
       </c>
@@ -7406,8 +7618,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU54">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>68</v>
       </c>
@@ -7548,8 +7764,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU55">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="56" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>111</v>
       </c>
@@ -7623,7 +7843,7 @@
         <v>6</v>
       </c>
       <c r="Y56">
-        <f t="shared" ref="Y56:Y83" si="4">SUM(B56:X56)</f>
+        <f t="shared" ref="Y56:Y83" si="5">SUM(B56:X56)</f>
         <v>33</v>
       </c>
       <c r="Z56" t="s">
@@ -7690,8 +7910,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU56">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
     </row>
-    <row r="57" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>70</v>
       </c>
@@ -7765,7 +7989,7 @@
         <v>2</v>
       </c>
       <c r="Y57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>44</v>
       </c>
       <c r="Z57" t="s">
@@ -7832,8 +8056,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU57">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
     </row>
-    <row r="58" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>112</v>
       </c>
@@ -7970,8 +8198,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="AU58">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="59" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>71</v>
       </c>
@@ -8045,7 +8277,7 @@
         <v>12</v>
       </c>
       <c r="Y59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Z59" t="s">
@@ -8112,8 +8344,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="AU59">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="60" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>113</v>
       </c>
@@ -8165,8 +8401,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU60">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>114</v>
       </c>
@@ -8304,8 +8544,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="AU61">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="62" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>72</v>
       </c>
@@ -8313,8 +8557,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="63" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>115</v>
       </c>
@@ -8451,8 +8699,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="AU63">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>73</v>
       </c>
@@ -8526,7 +8778,7 @@
         <v>12</v>
       </c>
       <c r="Y64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="Z64" t="s">
@@ -8593,8 +8845,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AU64">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="65" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>122</v>
       </c>
@@ -8734,8 +8990,12 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
+      <c r="AU65">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="66" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>74</v>
       </c>
@@ -8809,7 +9069,7 @@
         <v>21</v>
       </c>
       <c r="Y66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>103</v>
       </c>
       <c r="Z66" t="s">
@@ -8876,8 +9136,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="AU66">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
     </row>
-    <row r="67" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>75</v>
       </c>
@@ -8951,7 +9215,7 @@
         <v>12</v>
       </c>
       <c r="Y67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="Z67" t="s">
@@ -9018,8 +9282,12 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="AU67">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
     </row>
-    <row r="68" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>116</v>
       </c>
@@ -9153,12 +9421,16 @@
         <v>12</v>
       </c>
       <c r="AT68">
-        <f t="shared" ref="AT68:AT83" si="5">SUM(Z68:AS68)</f>
+        <f t="shared" ref="AT68:AT83" si="6">SUM(Z68:AS68)</f>
+        <v>1</v>
+      </c>
+      <c r="AU68">
+        <f t="shared" ref="AU68:AU83" si="7">SUM(Y68,AT68)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
+    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B69" t="s">
@@ -9294,585 +9566,609 @@
         <v>12</v>
       </c>
       <c r="AT69">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="AU69">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70">
+        <v>7</v>
+      </c>
+      <c r="E70" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" t="s">
+        <v>12</v>
+      </c>
+      <c r="H70" t="s">
+        <v>12</v>
+      </c>
+      <c r="I70" t="s">
+        <v>12</v>
+      </c>
+      <c r="J70">
+        <v>2</v>
+      </c>
+      <c r="K70" t="s">
+        <v>12</v>
+      </c>
+      <c r="L70" t="s">
+        <v>12</v>
+      </c>
+      <c r="M70" t="s">
+        <v>12</v>
+      </c>
+      <c r="N70">
+        <v>4</v>
+      </c>
+      <c r="O70" t="s">
+        <v>12</v>
+      </c>
+      <c r="P70" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>12</v>
+      </c>
+      <c r="R70" t="s">
+        <v>12</v>
+      </c>
+      <c r="S70" t="s">
+        <v>12</v>
+      </c>
+      <c r="T70" t="s">
+        <v>12</v>
+      </c>
+      <c r="U70" t="s">
+        <v>12</v>
+      </c>
+      <c r="V70" t="s">
+        <v>12</v>
+      </c>
+      <c r="W70">
+        <v>1</v>
+      </c>
+      <c r="X70" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y70">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="Z70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB70">
+        <v>1</v>
+      </c>
+      <c r="AC70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH70">
+        <v>1</v>
+      </c>
+      <c r="AI70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK70">
+        <v>1</v>
+      </c>
+      <c r="AL70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AR70">
+        <v>4</v>
+      </c>
+      <c r="AS70" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT70">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="AU70">
+        <f t="shared" si="7"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="V71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="W71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="X71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y71" s="2"/>
+      <c r="Z71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AR71" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS71" s="2">
+        <v>2</v>
+      </c>
+      <c r="AT71">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="AU71">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT72">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AU72">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" t="s">
+        <v>12</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" t="s">
+        <v>12</v>
+      </c>
+      <c r="H73" t="s">
+        <v>12</v>
+      </c>
+      <c r="I73" t="s">
+        <v>12</v>
+      </c>
+      <c r="J73" t="s">
+        <v>12</v>
+      </c>
+      <c r="K73" t="s">
+        <v>12</v>
+      </c>
+      <c r="L73" t="s">
+        <v>12</v>
+      </c>
+      <c r="M73" t="s">
+        <v>12</v>
+      </c>
+      <c r="N73" t="s">
+        <v>12</v>
+      </c>
+      <c r="O73" t="s">
+        <v>12</v>
+      </c>
+      <c r="P73" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>12</v>
+      </c>
+      <c r="R73">
+        <v>1</v>
+      </c>
+      <c r="S73" t="s">
+        <v>12</v>
+      </c>
+      <c r="T73" t="s">
+        <v>12</v>
+      </c>
+      <c r="U73" t="s">
+        <v>12</v>
+      </c>
+      <c r="V73" t="s">
+        <v>12</v>
+      </c>
+      <c r="W73" t="s">
+        <v>12</v>
+      </c>
+      <c r="X73" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y73">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
+      <c r="Z73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AR73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS73" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT73">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AU73">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="70" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B70" t="s">
-        <v>12</v>
-      </c>
-      <c r="C70" t="s">
-        <v>12</v>
-      </c>
-      <c r="D70">
-        <v>7</v>
-      </c>
-      <c r="E70" t="s">
-        <v>12</v>
-      </c>
-      <c r="F70" t="s">
-        <v>12</v>
-      </c>
-      <c r="G70" t="s">
-        <v>12</v>
-      </c>
-      <c r="H70" t="s">
-        <v>12</v>
-      </c>
-      <c r="I70" t="s">
-        <v>12</v>
-      </c>
-      <c r="J70">
-        <v>2</v>
-      </c>
-      <c r="K70" t="s">
-        <v>12</v>
-      </c>
-      <c r="L70" t="s">
-        <v>12</v>
-      </c>
-      <c r="M70" t="s">
-        <v>12</v>
-      </c>
-      <c r="N70">
-        <v>4</v>
-      </c>
-      <c r="O70" t="s">
-        <v>12</v>
-      </c>
-      <c r="P70" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>12</v>
-      </c>
-      <c r="R70" t="s">
-        <v>12</v>
-      </c>
-      <c r="S70" t="s">
-        <v>12</v>
-      </c>
-      <c r="T70" t="s">
-        <v>12</v>
-      </c>
-      <c r="U70" t="s">
-        <v>12</v>
-      </c>
-      <c r="V70" t="s">
-        <v>12</v>
-      </c>
-      <c r="W70">
-        <v>1</v>
-      </c>
-      <c r="X70" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y70">
-        <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="Z70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB70">
-        <v>1</v>
-      </c>
-      <c r="AC70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AH70">
-        <v>1</v>
-      </c>
-      <c r="AI70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK70">
-        <v>1</v>
-      </c>
-      <c r="AL70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AM70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AQ70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AR70">
-        <v>4</v>
-      </c>
-      <c r="AS70" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT70">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="T71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="U71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="V71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="W71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="X71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y71" s="2"/>
-      <c r="Z71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AH71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AM71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AQ71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AR71" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS71" s="2">
-        <v>2</v>
-      </c>
-      <c r="AT71">
+    <row r="74" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B74" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74" t="s">
+        <v>12</v>
+      </c>
+      <c r="G74" t="s">
+        <v>12</v>
+      </c>
+      <c r="H74" t="s">
+        <v>12</v>
+      </c>
+      <c r="I74" t="s">
+        <v>12</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74" t="s">
+        <v>12</v>
+      </c>
+      <c r="L74" t="s">
+        <v>12</v>
+      </c>
+      <c r="M74" t="s">
+        <v>12</v>
+      </c>
+      <c r="N74" t="s">
+        <v>12</v>
+      </c>
+      <c r="O74" t="s">
+        <v>12</v>
+      </c>
+      <c r="P74" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>12</v>
+      </c>
+      <c r="R74" t="s">
+        <v>12</v>
+      </c>
+      <c r="S74" t="s">
+        <v>12</v>
+      </c>
+      <c r="T74" t="s">
+        <v>12</v>
+      </c>
+      <c r="U74" t="s">
+        <v>12</v>
+      </c>
+      <c r="V74" t="s">
+        <v>12</v>
+      </c>
+      <c r="W74" t="s">
+        <v>12</v>
+      </c>
+      <c r="X74" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y74">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
+      <c r="Z74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AR74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS74" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT74">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AU74">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="72" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AT72">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B73" t="s">
-        <v>12</v>
-      </c>
-      <c r="C73" t="s">
-        <v>12</v>
-      </c>
-      <c r="D73" t="s">
-        <v>12</v>
-      </c>
-      <c r="E73">
-        <v>1</v>
-      </c>
-      <c r="F73" t="s">
-        <v>12</v>
-      </c>
-      <c r="G73" t="s">
-        <v>12</v>
-      </c>
-      <c r="H73" t="s">
-        <v>12</v>
-      </c>
-      <c r="I73" t="s">
-        <v>12</v>
-      </c>
-      <c r="J73" t="s">
-        <v>12</v>
-      </c>
-      <c r="K73" t="s">
-        <v>12</v>
-      </c>
-      <c r="L73" t="s">
-        <v>12</v>
-      </c>
-      <c r="M73" t="s">
-        <v>12</v>
-      </c>
-      <c r="N73" t="s">
-        <v>12</v>
-      </c>
-      <c r="O73" t="s">
-        <v>12</v>
-      </c>
-      <c r="P73" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q73" t="s">
-        <v>12</v>
-      </c>
-      <c r="R73">
-        <v>1</v>
-      </c>
-      <c r="S73" t="s">
-        <v>12</v>
-      </c>
-      <c r="T73" t="s">
-        <v>12</v>
-      </c>
-      <c r="U73" t="s">
-        <v>12</v>
-      </c>
-      <c r="V73" t="s">
-        <v>12</v>
-      </c>
-      <c r="W73" t="s">
-        <v>12</v>
-      </c>
-      <c r="X73" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y73">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="Z73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AH73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AM73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AQ73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AR73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS73" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT73">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B74" t="s">
-        <v>12</v>
-      </c>
-      <c r="C74" t="s">
-        <v>12</v>
-      </c>
-      <c r="D74">
-        <v>1</v>
-      </c>
-      <c r="E74" t="s">
-        <v>12</v>
-      </c>
-      <c r="F74" t="s">
-        <v>12</v>
-      </c>
-      <c r="G74" t="s">
-        <v>12</v>
-      </c>
-      <c r="H74" t="s">
-        <v>12</v>
-      </c>
-      <c r="I74" t="s">
-        <v>12</v>
-      </c>
-      <c r="J74">
-        <v>1</v>
-      </c>
-      <c r="K74" t="s">
-        <v>12</v>
-      </c>
-      <c r="L74" t="s">
-        <v>12</v>
-      </c>
-      <c r="M74" t="s">
-        <v>12</v>
-      </c>
-      <c r="N74" t="s">
-        <v>12</v>
-      </c>
-      <c r="O74" t="s">
-        <v>12</v>
-      </c>
-      <c r="P74" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q74" t="s">
-        <v>12</v>
-      </c>
-      <c r="R74" t="s">
-        <v>12</v>
-      </c>
-      <c r="S74" t="s">
-        <v>12</v>
-      </c>
-      <c r="T74" t="s">
-        <v>12</v>
-      </c>
-      <c r="U74" t="s">
-        <v>12</v>
-      </c>
-      <c r="V74" t="s">
-        <v>12</v>
-      </c>
-      <c r="W74" t="s">
-        <v>12</v>
-      </c>
-      <c r="X74" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y74">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="Z74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AH74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AM74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AQ74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AR74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS74" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT74">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>81</v>
       </c>
@@ -9946,7 +10242,7 @@
         <v>12</v>
       </c>
       <c r="Y75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Z75" t="s">
@@ -10010,11 +10306,15 @@
         <v>12</v>
       </c>
       <c r="AT75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AU75">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>118</v>
       </c>
@@ -10145,11 +10445,15 @@
         <v>1</v>
       </c>
       <c r="AT76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AU76">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>82</v>
       </c>
@@ -10223,7 +10527,7 @@
         <v>12</v>
       </c>
       <c r="Y77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="Z77" t="s">
@@ -10287,11 +10591,15 @@
         <v>12</v>
       </c>
       <c r="AT77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AU77">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="78" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>119</v>
       </c>
@@ -10425,11 +10733,15 @@
         <v>12</v>
       </c>
       <c r="AT78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AU78">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>83</v>
       </c>
@@ -10503,7 +10815,7 @@
         <v>12</v>
       </c>
       <c r="Y79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="Z79" t="s">
@@ -10567,11 +10879,15 @@
         <v>12</v>
       </c>
       <c r="AT79">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AU79">
+        <f t="shared" si="7"/>
+        <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>84</v>
       </c>
@@ -10645,7 +10961,7 @@
         <v>3</v>
       </c>
       <c r="Y80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="Z80" t="s">
@@ -10709,11 +11025,15 @@
         <v>12</v>
       </c>
       <c r="AT80">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AU80">
+        <f t="shared" si="7"/>
+        <v>30</v>
       </c>
     </row>
-    <row r="81" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>85</v>
       </c>
@@ -10787,7 +11107,7 @@
         <v>12</v>
       </c>
       <c r="Y81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>47</v>
       </c>
       <c r="Z81" t="s">
@@ -10851,11 +11171,15 @@
         <v>12</v>
       </c>
       <c r="AT81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
+      <c r="AU81">
+        <f t="shared" si="7"/>
+        <v>49</v>
+      </c>
     </row>
-    <row r="82" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>86</v>
       </c>
@@ -10929,7 +11253,7 @@
         <v>1</v>
       </c>
       <c r="Y82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="Z82" t="s">
@@ -10993,11 +11317,15 @@
         <v>12</v>
       </c>
       <c r="AT82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="AU82">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
     </row>
-    <row r="83" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>87</v>
       </c>
@@ -11071,7 +11399,7 @@
         <v>1</v>
       </c>
       <c r="Y83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="Z83" t="s">
@@ -11135,108 +11463,112 @@
         <v>12</v>
       </c>
       <c r="AT83">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AU83">
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B84">
-        <f t="shared" ref="B84:Y84" si="6">SUM(B3:B83)</f>
+        <f t="shared" ref="B84:Y84" si="8">SUM(B3:B83)</f>
         <v>2</v>
       </c>
       <c r="C84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="D84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>97</v>
       </c>
       <c r="E84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="G84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>58</v>
       </c>
       <c r="H84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="I84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="J84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>67</v>
       </c>
       <c r="K84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>28</v>
       </c>
       <c r="L84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="M84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="N84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>42</v>
       </c>
       <c r="O84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="P84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="Q84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>113</v>
       </c>
       <c r="R84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="S84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="T84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="U84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>74</v>
       </c>
       <c r="V84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>97</v>
       </c>
       <c r="W84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>38</v>
       </c>
       <c r="X84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>83</v>
       </c>
       <c r="Y84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>799</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added plate and distributions
</commit_message>
<xml_diff>
--- a/Data/Skyros List.xlsx
+++ b/Data/Skyros List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eranee\Desktop\Beetles\RScripts\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695D0A7C-AB68-4D39-A17A-E7E0E5F3B9AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F08C857-B254-45CA-B594-535EE3D9A321}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{983DCE97-DC4A-4F6A-9F48-E813D0A7A667}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2986" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3019" uniqueCount="153">
   <si>
     <t>Omaliinae</t>
   </si>
@@ -457,6 +457,42 @@
   </si>
   <si>
     <t>Middle-european/mediterranian</t>
+  </si>
+  <si>
+    <t>European</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palaearctic </t>
+  </si>
+  <si>
+    <t>Middle eastern/caucasic</t>
+  </si>
+  <si>
+    <t>European/Russian</t>
+  </si>
+  <si>
+    <t>Western european</t>
+  </si>
+  <si>
+    <t>Mediterranian/middle eastern</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t>Endemic?</t>
+  </si>
+  <si>
+    <t>European/Middle-eastern</t>
+  </si>
+  <si>
+    <t>European/Caucasus</t>
+  </si>
+  <si>
+    <t>European/mediterranian</t>
+  </si>
+  <si>
+    <t>Greece/Turkey/Lebanon/Israel</t>
   </si>
 </sst>
 </file>
@@ -829,10 +865,10 @@
   <dimension ref="A1:AV84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AE21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AE58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AV46" sqref="AV46"/>
+      <selection pane="bottomRight" activeCell="AV74" sqref="AV74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6875,6 +6911,9 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="AV46" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="47" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
@@ -7021,6 +7060,9 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
+      <c r="AV47" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="48" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
@@ -7167,8 +7209,11 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="AV48" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="49" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>56</v>
       </c>
@@ -7313,8 +7358,11 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="AV49" t="s">
+        <v>141</v>
+      </c>
     </row>
-    <row r="50" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
@@ -7459,8 +7507,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AV50" t="s">
+        <v>141</v>
+      </c>
     </row>
-    <row r="51" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>58</v>
       </c>
@@ -7474,7 +7525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>59</v>
       </c>
@@ -7619,8 +7670,11 @@
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
+      <c r="AV52" t="s">
+        <v>131</v>
+      </c>
     </row>
-    <row r="53" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>62</v>
       </c>
@@ -7765,8 +7819,11 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
+      <c r="AV53" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="54" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>66</v>
       </c>
@@ -7780,7 +7837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>67</v>
       </c>
@@ -7925,8 +7982,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AV55" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="56" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>110</v>
       </c>
@@ -8071,8 +8131,11 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
+      <c r="AV56" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="57" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>69</v>
       </c>
@@ -8217,8 +8280,11 @@
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
+      <c r="AV57" t="s">
+        <v>131</v>
+      </c>
     </row>
-    <row r="58" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>111</v>
       </c>
@@ -8359,8 +8425,11 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
+      <c r="AV58" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="59" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>70</v>
       </c>
@@ -8505,8 +8574,11 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
+      <c r="AV59" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="60" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>112</v>
       </c>
@@ -8563,7 +8635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>113</v>
       </c>
@@ -8705,8 +8777,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AV61" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="62" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>71</v>
       </c>
@@ -8719,7 +8794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>114</v>
       </c>
@@ -8860,8 +8935,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AV63" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="64" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>72</v>
       </c>
@@ -9006,8 +9084,11 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
+      <c r="AV64" t="s">
+        <v>131</v>
+      </c>
     </row>
-    <row r="65" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>121</v>
       </c>
@@ -9151,8 +9232,11 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="AV65" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="66" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>73</v>
       </c>
@@ -9297,8 +9381,11 @@
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
+      <c r="AV66" t="s">
+        <v>146</v>
+      </c>
     </row>
-    <row r="67" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>74</v>
       </c>
@@ -9443,8 +9530,11 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
+      <c r="AV67" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="68" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>115</v>
       </c>
@@ -9585,8 +9675,11 @@
         <f t="shared" ref="AU68:AU83" si="7">SUM(Y68,AT68)</f>
         <v>1</v>
       </c>
+      <c r="AV68" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="69" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>126</v>
       </c>
@@ -9730,8 +9823,11 @@
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
+      <c r="AV69" t="s">
+        <v>147</v>
+      </c>
     </row>
-    <row r="70" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>75</v>
       </c>
@@ -9876,8 +9972,11 @@
         <f t="shared" si="7"/>
         <v>21</v>
       </c>
+      <c r="AV70" s="1" t="s">
+        <v>148</v>
+      </c>
     </row>
-    <row r="71" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>116</v>
       </c>
@@ -10019,8 +10118,11 @@
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
+      <c r="AV71" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="72" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>76</v>
       </c>
@@ -10033,7 +10135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>78</v>
       </c>
@@ -10178,8 +10280,11 @@
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
+      <c r="AV73" t="s">
+        <v>149</v>
+      </c>
     </row>
-    <row r="74" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>79</v>
       </c>
@@ -10324,8 +10429,11 @@
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
+      <c r="AV74" t="s">
+        <v>131</v>
+      </c>
     </row>
-    <row r="75" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>80</v>
       </c>
@@ -10470,8 +10578,11 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
+      <c r="AV75" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="76" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>117</v>
       </c>
@@ -10609,8 +10720,11 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
+      <c r="AV76" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="77" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>81</v>
       </c>
@@ -10755,8 +10869,11 @@
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
+      <c r="AV77" t="s">
+        <v>149</v>
+      </c>
     </row>
-    <row r="78" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>118</v>
       </c>
@@ -10897,8 +11014,11 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
+      <c r="AV78" t="s">
+        <v>131</v>
+      </c>
     </row>
-    <row r="79" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>82</v>
       </c>
@@ -11043,8 +11163,11 @@
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
+      <c r="AV79" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="80" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>83</v>
       </c>
@@ -11189,8 +11312,11 @@
         <f t="shared" si="7"/>
         <v>30</v>
       </c>
+      <c r="AV80" t="s">
+        <v>150</v>
+      </c>
     </row>
-    <row r="81" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>84</v>
       </c>
@@ -11335,8 +11461,11 @@
         <f t="shared" si="7"/>
         <v>49</v>
       </c>
+      <c r="AV81" t="s">
+        <v>151</v>
+      </c>
     </row>
-    <row r="82" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>85</v>
       </c>
@@ -11481,8 +11610,11 @@
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
+      <c r="AV82" t="s">
+        <v>152</v>
+      </c>
     </row>
-    <row r="83" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>86</v>
       </c>
@@ -11627,8 +11759,11 @@
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
+      <c r="AV83" t="s">
+        <v>131</v>
+      </c>
     </row>
-    <row r="84" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>87</v>
       </c>
@@ -11732,6 +11867,6 @@
   </sheetData>
   <autoFilter ref="A1:AT84" xr:uid="{CE19B23F-E421-4726-B0AC-440FEEAF8EFE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>